<commit_message>
Added poldScenarios array objects to scripts.js, ready to start logic
</commit_message>
<xml_diff>
--- a/sites/packing-for-peanuts/pold-box-scenarios.xlsx
+++ b/sites/packing-for-peanuts/pold-box-scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessel\Documents\GitHub\scene_selection\sites\packing-for-peanuts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesselafica/sites/scene_selection/sites/packing-for-peanuts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3F14913-6351-438F-BFA7-0616B1F67479}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02876684-5A0B-0347-AD7B-FE6A899FB635}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29535" yWindow="735" windowWidth="10155" windowHeight="12795" xr2:uid="{DBCE36A3-1415-46AF-9B5E-B5762E034471}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{DBCE36A3-1415-46AF-9B5E-B5762E034471}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>POLD Box Shipping Scenarios</t>
   </si>
@@ -51,9 +45,6 @@
     <t>Scenario 1</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Scenario 2</t>
   </si>
   <si>
@@ -66,9 +57,6 @@
     <t>Scenario 5</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Scenario 6</t>
   </si>
   <si>
@@ -91,6 +79,132 @@
   </si>
   <si>
     <t>Scenario 13</t>
+  </si>
+  <si>
+    <t>{
+    api    : 0,
+    pold   : 18,
+    ssr    : 0,
+    poldSsr: 18,
+    recirc : 1
+  },</t>
+  </si>
+  <si>
+    <t>{
+api : 3,
+pold : 0,
+ssr : 0,
+poldSsr : 0,
+recirc : 3
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 0,
+pold : 0,
+ssr : 2,
+poldSsr : 1,
+recirc : 5
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 6,
+pold : 0,
+ssr : 2,
+poldSsr : 1,
+recirc : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 2,
+pold : 2,
+ssr : 2,
+poldSsr : 3,
+recirc : 3
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 1,
+pold : 4,
+ssr : 2,
+poldSsr : 5,
+recirc : 3
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 0,
+pold : 6,
+ssr : 2,
+poldSsr : 7,
+recirc : 3
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 0,
+pold : 15,
+ssr : 2,
+poldSsr : 16,
+recirc : 2
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 0,
+pold : 22,
+ssr : 2,
+poldSsr : 23,
+recirc : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 2,
+pold : 14,
+ssr : 2,
+poldSsr : 15,
+recirc : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 1,
+pold : 18,
+ssr : 2,
+poldSsr : 19,
+recirc : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 3,
+pold : 12,
+ssr : 2,
+poldSsr : 13,
+recirc : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 4,
+pold : 8,
+ssr : 2,
+poldSsr : 9,
+recirc : 0
+}</t>
+  </si>
+  <si>
+    <t>{
+api : 5,
+pold : 4,
+ssr : 2,
+poldSsr : 5,
+recirc : 0
+}</t>
   </si>
 </sst>
 </file>
@@ -126,8 +240,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,18 +560,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA31AFA7-55E0-499A-B4F0-75E8B80A3DE3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="35.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -481,16 +601,29 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>CONCATENATE("{",CHAR(10),"api : ",B2,",",CHAR(10),"pold : ",C2,",",CHAR(10),"ssr : ",D2,",",CHAR(10),"poldSsr : ",SUM(C2+(D2/2)),",",CHAR(10),"recirc : ",E2,CHAR(10),"}")</f>
+        <v>{
+api : 3,
+pold : 0,
+ssr : 0,
+poldSsr : 0,
+recirc : 3
+}</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -498,16 +631,29 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="D3">
+        <v>2</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:G15" si="0">CONCATENATE("{",CHAR(10),"api : ",B3,",",CHAR(10),"pold : ",C3,",",CHAR(10),"ssr : ",D3,",",CHAR(10),"poldSsr : ",SUM(C3+(D3/2)),",",CHAR(10),"recirc : ",E3,CHAR(10),"}")</f>
+        <v>{
+api : 0,
+pold : 0,
+ssr : 2,
+poldSsr : 1,
+recirc : 5
+}</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -515,16 +661,29 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
+      <c r="D4">
+        <v>2</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 6,
+pold : 0,
+ssr : 2,
+poldSsr : 1,
+recirc : 0
+}</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -532,16 +691,29 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
+      <c r="D5">
+        <v>2</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 2,
+pold : 2,
+ssr : 2,
+poldSsr : 3,
+recirc : 3
+}</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -549,16 +721,29 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
+      <c r="D6">
+        <v>2</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 1,
+pold : 4,
+ssr : 2,
+poldSsr : 5,
+recirc : 3
+}</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -566,16 +751,29 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
+      <c r="D7">
+        <v>2</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 0,
+pold : 6,
+ssr : 2,
+poldSsr : 7,
+recirc : 3
+}</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -583,16 +781,29 @@
       <c r="C8">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
+      <c r="D8">
+        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 0,
+pold : 15,
+ssr : 2,
+poldSsr : 16,
+recirc : 2
+}</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -600,16 +811,29 @@
       <c r="C9">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
+      <c r="D9">
+        <v>2</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 0,
+pold : 22,
+ssr : 2,
+poldSsr : 23,
+recirc : 0
+}</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -617,16 +841,29 @@
       <c r="C10">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
+      <c r="D10">
+        <v>2</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 2,
+pold : 14,
+ssr : 2,
+poldSsr : 15,
+recirc : 0
+}</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -634,16 +871,29 @@
       <c r="C11">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
-        <v>6</v>
+      <c r="D11">
+        <v>2</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 1,
+pold : 18,
+ssr : 2,
+poldSsr : 19,
+recirc : 0
+}</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -651,16 +901,29 @@
       <c r="C12">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
+      <c r="D12">
+        <v>2</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 3,
+pold : 12,
+ssr : 2,
+poldSsr : 13,
+recirc : 0
+}</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -668,16 +931,29 @@
       <c r="C13">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
+      <c r="D13">
+        <v>2</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 4,
+pold : 8,
+ssr : 2,
+poldSsr : 9,
+recirc : 0
+}</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -685,11 +961,42 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>6</v>
+      <c r="D14">
+        <v>2</v>
       </c>
       <c r="E14">
         <v>0</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : 5,
+pold : 4,
+ssr : 2,
+poldSsr : 5,
+recirc : 0
+}</v>
+      </c>
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>{
+api : ,
+pold : ,
+ssr : 2,
+poldSsr : 1,
+recirc : 
+}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>